<commit_message>
Fixed a formatting issue in the data tests
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth/4_descricao/descricao.xlsx
+++ b/input_data/data_ground_truth/4_descricao/descricao.xlsx
@@ -151,10 +151,10 @@
     <t>Capacidade do sistema socioecológico de se preparar e se ajustar às alterações climáticas ou aos danos climáticos potenciais relacionados à seca, principalmente para diminuir os impactos negativos, aproveitar as oportunidades ou responder às consequências. O Índice de Capacidade Adaptativa é resultante da composição dos indicadores temáticos: logística da produção e abastecimento, planejamento e gestão da segurança alimentar e nutricional, manutenção da produção agropecuária, e capacidade socioeconômica familiar.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;ADGER, W. N. Vulnerability. Global Environmental Change, v. 16, n. 3, p. 268–281, ago. 2006.&lt;br&gt;GALLOPÍN, G. C.. Box 1: A systemic synthesis of the relations between vulnerability, hazard, exposure and impact, aimed at policy identification. In: Economic Commission for Latin American and the Caribbean (ECLAC). Handbook for Estimating the Socio-Economic and Environmental Effects of Disasters. Mexico, D.F.: ECLAC, LC/MEX/G.S., p. 2-5, 2003.&lt;br&gt;GALLOPÍN, G. C.. Linkages between vulnerability, resilience, and adaptive capacity. Global Environmental Change, v. 16, p. 293-303, 2006.&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp.</t>
   </si>
   <si>
-    <t>Produção e comercialização</t>
+    <t>Produção e Comercialização</t>
   </si>
   <si>
-    <t>Produção e comercialização de alimentos</t>
+    <t>Produção e Comercialização de Alimentos</t>
   </si>
   <si>
     <t>Sensibilidade do sistema socioecológico quanto à disponibilidade de alimento e as possíveis limitações na sua comercialização no presente e no futuro considerando uma situação de seca</t>
@@ -163,10 +163,10 @@
     <t>Sensibilidade do sistema quanto à disponibilidade de alimento e as possíveis limitações na sua comercialização no presente e no futuro considerando uma situação de seca. Essa informação é resultante da composição dos indicadores: baixa produção de alimentos básicos e não diversificação da produção local.&lt;br&gt;&lt;br&gt;Fonte:&lt;br&gt;Sistema de Informações e Análises sobre Impactos das Mudanças Climáticas – AdaptaBrasil MCTI.</t>
   </si>
   <si>
-    <t>Produtores e estabelecimentos agropecuários</t>
+    <t>Produtores e Estabelecimentos Agropecuários</t>
   </si>
   <si>
-    <t>Características dos produtores e dos estabelecimentos agropecuários</t>
+    <t>Características dos Produtores e dos Estabelecimentos Agropecuários</t>
   </si>
   <si>
     <t>Dependência dos estabelecimentos agropecuários aos aspectos que podem expressar a sensibilidade do sistema em situação de seca</t>

</xml_diff>